<commit_message>
Antimicrobial H2O cackra C new analysis.
</commit_message>
<xml_diff>
--- a/Data/Antimicrobial_H2O_Chakra_C.xlsx
+++ b/Data/Antimicrobial_H2O_Chakra_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4ss0\Documents\Ikiam21062022\Proyecto Guayusa\Antimicrobial_I_guayusa\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F38CE5-C19E-48C3-BE9D-EE27B65FE99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEC3DB8-4768-4116-AD2A-F3798F3181CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Escalas" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51317C54-FA6A-412C-98DB-C8D1CBD7C6B3}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1292,7 +1292,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4:S6"/>
+      <selection activeCell="E4" sqref="E4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2585,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8542F08-6268-4576-8880-7C096C0A263D}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2614,7 +2614,8 @@
         <v>6.0271976948900763</v>
       </c>
       <c r="B2">
-        <v>24.514317574558454</v>
+        <f>AVERAGE(B3:B4)</f>
+        <v>24.446517568801305</v>
       </c>
       <c r="C2">
         <v>7.0432428515887358</v>
@@ -2634,7 +2635,7 @@
         <v>5.9590793792467451</v>
       </c>
       <c r="B3">
-        <v>24.378717563044159</v>
+        <v>24.514317574558454</v>
       </c>
       <c r="C3">
         <v>6.9751245359454055</v>
@@ -2654,7 +2655,7 @@
         <v>6.0271976948900763</v>
       </c>
       <c r="B4">
-        <v>25.327917643644223</v>
+        <v>24.378717563044159</v>
       </c>
       <c r="C4">
         <v>7.2460062490878112</v>
@@ -2678,7 +2679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A44E2461-B251-4167-A77E-89B4563C0871}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>